<commit_message>
login success handler corrigé et template de home modifiée
</commit_message>
<xml_diff>
--- a/public/exports/users.xlsx
+++ b/public/exports/users.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Nom Utilisateur</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>Chayma.Hassayoun@esprit.tn</t>
+  </si>
+  <si>
+    <t>chaymaaa</t>
+  </si>
+  <si>
+    <t>chachahassayoun@gmail.com</t>
+  </si>
+  <si>
+    <t>hassayoune</t>
   </si>
 </sst>
 </file>
@@ -436,7 +445,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="E15" sqref="E15"/>
@@ -507,6 +516,20 @@
         <v>12345678</v>
       </c>
     </row>
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>54224709</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>